<commit_message>
Changes of unit_capacities on first sheet
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/Products/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/Products/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\ammonia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/Products/ammonia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A398C2-2803-4388-96E0-F2CB59F35ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{51A398C2-2803-4388-96E0-F2CB59F35ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72167D49-2E47-47B9-B810-8C3D649E95BC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="113">
   <si>
     <t>Unit</t>
   </si>
@@ -293,9 +293,6 @@
   </si>
   <si>
     <t>water</t>
-  </si>
-  <si>
-    <t>steam_plant</t>
   </si>
   <si>
     <t>h2</t>
@@ -525,6 +522,20 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -559,20 +570,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1287,11 +1284,11 @@
     <tableColumn id="10" xr3:uid="{CD6FCAF1-2543-4CF8-99F5-E24DBA2DEDC0}" name="Output4" dataDxfId="10"/>
     <tableColumn id="11" xr3:uid="{88F2DAC4-E2C3-4C34-B709-2523E8BE5B1F}" name="Relation_In1_In2" dataDxfId="9"/>
     <tableColumn id="14" xr3:uid="{3C190E97-FD9A-4F36-8EBF-717B1ECA00B1}" name="Relation_In1_In3" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{043147D8-AE82-457E-8F19-EB4AE9D43B9E}" name="Relation_In1_In4" dataDxfId="0"/>
-    <tableColumn id="12" xr3:uid="{A190E492-7FDF-403D-B8AF-17448A48E47F}" name="Relation_In1_Out1" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{26E8D274-C985-4E20-8920-2BAC0A372552}" name="Relation_Out1_Out2" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{4E0BCAE8-11F8-4D98-AECC-86C8A3C2B5C1}" name="Relation_Out1_Out3" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{3C0369D5-4DD0-4B4B-9480-0C4665C0BC59}" name="Relation_Out1_Out4" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{043147D8-AE82-457E-8F19-EB4AE9D43B9E}" name="Relation_In1_In4" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{A190E492-7FDF-403D-B8AF-17448A48E47F}" name="Relation_In1_Out1" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{26E8D274-C985-4E20-8920-2BAC0A372552}" name="Relation_Out1_Out2" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{4E0BCAE8-11F8-4D98-AECC-86C8A3C2B5C1}" name="Relation_Out1_Out3" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{3C0369D5-4DD0-4B4B-9480-0C4665C0BC59}" name="Relation_Out1_Out4" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1307,7 +1304,7 @@
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -1326,7 +1323,7 @@
     <tableColumn id="21" xr3:uid="{EC2CC790-C17D-4744-A981-3984808E5B33}" name="vom_cost_Input2"/>
     <tableColumn id="24" xr3:uid="{41B338E4-2058-41E9-8000-97D77450FBC3}" name="vom_cost_Output1"/>
     <tableColumn id="25" xr3:uid="{DDAFCF0A-1EF1-4B7B-9742-01F9FA7A22E5}" name="vom_cost_Output2"/>
-    <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime" dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime" dataDxfId="1"/>
     <tableColumn id="30" xr3:uid="{09434E4A-7BF5-4547-9708-EA3F0F7ADC8E}" name="initial_connections_invested_available"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1337,7 +1334,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:K5" totalsRowShown="0">
   <autoFilter ref="A1:K5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{8C29206C-8DC6-44DB-A8D1-3D5625C277AD}" name="Object_type"/>
@@ -1665,7 +1662,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z18" sqref="Z18"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1691,7 +1688,7 @@
         <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -1700,16 +1697,16 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" t="s">
         <v>98</v>
       </c>
-      <c r="G1" t="s">
-        <v>99</v>
-      </c>
       <c r="H1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J1" t="s">
         <v>61</v>
@@ -1736,7 +1733,7 @@
         <v>41</v>
       </c>
       <c r="R1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -1754,7 +1751,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
@@ -1767,7 +1764,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>60</v>
@@ -1780,7 +1777,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
         <v>57</v>
@@ -1802,61 +1799,45 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
         <v>102</v>
       </c>
-      <c r="B6" t="s">
-        <v>103</v>
-      </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="M8">
-        <v>0.11929223744292237</v>
+        <v>72</v>
+      </c>
+      <c r="N8">
+        <v>1.4865951742627345E-3</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" t="s">
-        <v>72</v>
-      </c>
-      <c r="N9">
-        <v>1.4865951742627345E-3</v>
-      </c>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="P11" s="1"/>
@@ -1869,7 +1850,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P9 P11:P12" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P11:P12 P2:P8" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
       <formula1>"h, D, W, M, Q, Y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1885,7 +1866,7 @@
           <x14:formula1>
             <xm:f>Drop_Down!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B11:B1048576 B1:B9</xm:sqref>
+          <xm:sqref>B11:B1048576 B1:B8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1922,10 +1903,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
@@ -1934,31 +1915,31 @@
         <v>4</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -1988,7 +1969,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>59</v>
@@ -2013,7 +1994,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>60</v>
@@ -2038,7 +2019,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>57</v>
@@ -2052,10 +2033,10 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -2073,10 +2054,10 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>67</v>
@@ -2085,10 +2066,10 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -2106,29 +2087,29 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7">
@@ -2151,13 +2132,13 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -2396,22 +2377,22 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
       </c>
       <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
         <v>74</v>
       </c>
-      <c r="D3" t="s">
-        <v>75</v>
-      </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s">
         <v>32</v>
@@ -2452,22 +2433,22 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
         <v>110</v>
       </c>
-      <c r="B4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" t="s">
-        <v>111</v>
-      </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
         <v>32</v>
@@ -2484,7 +2465,7 @@
         <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
         <v>71</v>
@@ -2596,7 +2577,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
@@ -2622,10 +2603,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2721,7 +2702,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
@@ -2751,7 +2732,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
@@ -2771,22 +2752,22 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed another column name problem
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/Products/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/Products/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/Products/ammonia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/Products/ammonia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{51A398C2-2803-4388-96E0-F2CB59F35ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72167D49-2E47-47B9-B810-8C3D649E95BC}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{51A398C2-2803-4388-96E0-F2CB59F35ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1B88561-2ACF-4BED-8233-B3D3F9BA2DD0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="3630" yWindow="-20490" windowWidth="25020" windowHeight="19680" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -462,7 +462,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -499,11 +499,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -516,11 +529,46 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1241,11 +1289,15 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:R11" totalsRowShown="0">
   <autoFilter ref="A1:R11" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
+    <tableColumn id="1" xr3:uid="{88DF4E3A-CD2C-432F-B85D-4C82436680EB}" name="Unit" dataDxfId="0"/>
     <tableColumn id="40" xr3:uid="{C2CFC5A4-5329-4F74-926A-18CEB18C062C}" name="Object_type"/>
     <tableColumn id="19" xr3:uid="{976E2DCC-BEF9-4E7C-96F4-92D75CC694A2}" name="unit_capacity"/>
     <tableColumn id="35" xr3:uid="{C3887B4E-C4A5-42AB-A92F-97AD44212E95}" name="mean_efficiency"/>
@@ -1260,8 +1312,8 @@
     <tableColumn id="12" xr3:uid="{F1A83AF0-CF23-4B00-9076-4E28DF8DAFD3}" name="fom_cost"/>
     <tableColumn id="21" xr3:uid="{400CD12D-8ADA-4557-B7CA-1464809EAFF0}" name="vom_cost"/>
     <tableColumn id="15" xr3:uid="{3F5A9F9C-E4A0-47A3-8DED-03601A5E69E7}" name="minimum_op_point"/>
-    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="26"/>
-    <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="25"/>
+    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="27"/>
+    <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="26"/>
     <tableColumn id="16" xr3:uid="{5F06ED78-6F41-4BEA-9209-36407E8BCFDC}" name="initial_units_on"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1269,26 +1321,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}" name="Table5" displayName="Table5" ref="A1:Q10" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}" name="Table5" displayName="Table5" ref="A1:Q10" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="A1:Q10" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{2BE3E317-773B-4E82-9035-69A43C6CB21B}" name="Unit" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{22613EE0-390D-4B04-9A9B-6D5554D1C8ED}" name="Object_type" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{54CD83B6-B63A-4ABD-99BD-9ED391BFB078}" name="Input1" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{F183F72C-A42E-4046-9CA2-B23C4DD3765C}" name="Input2" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{CA468CF3-FA3A-4DED-8C1A-ED8385FD2167}" name="Input3" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{6C9174ED-453E-45B1-B2C9-DC69B7CB535A}" name="Input4" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{513A63E4-7BE3-4AF5-AC5E-11EB4AF0D7AD}" name="Output1" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{4623E738-60A2-497B-BD61-91A608129A61}" name="Output2" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{5596B30B-5CDD-4E38-8C15-9C5F774E9B1F}" name="Output3" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{CD6FCAF1-2543-4CF8-99F5-E24DBA2DEDC0}" name="Output4" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{88F2DAC4-E2C3-4C34-B709-2523E8BE5B1F}" name="Relation_In1_In2" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{3C190E97-FD9A-4F36-8EBF-717B1ECA00B1}" name="Relation_In1_In3" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{043147D8-AE82-457E-8F19-EB4AE9D43B9E}" name="Relation_In1_In4" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{A190E492-7FDF-403D-B8AF-17448A48E47F}" name="Relation_In1_Out1" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{26E8D274-C985-4E20-8920-2BAC0A372552}" name="Relation_Out1_Out2" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{4E0BCAE8-11F8-4D98-AECC-86C8A3C2B5C1}" name="Relation_Out1_Out3" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{3C0369D5-4DD0-4B4B-9480-0C4665C0BC59}" name="Relation_Out1_Out4" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{2BE3E317-773B-4E82-9035-69A43C6CB21B}" name="Unit" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{22613EE0-390D-4B04-9A9B-6D5554D1C8ED}" name="Object_type" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{54CD83B6-B63A-4ABD-99BD-9ED391BFB078}" name="Input1" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{F183F72C-A42E-4046-9CA2-B23C4DD3765C}" name="Input2" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{CA468CF3-FA3A-4DED-8C1A-ED8385FD2167}" name="Input3" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{6C9174ED-453E-45B1-B2C9-DC69B7CB535A}" name="Input4" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{513A63E4-7BE3-4AF5-AC5E-11EB4AF0D7AD}" name="Output1" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{4623E738-60A2-497B-BD61-91A608129A61}" name="Output2" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{5596B30B-5CDD-4E38-8C15-9C5F774E9B1F}" name="Output3" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{CD6FCAF1-2543-4CF8-99F5-E24DBA2DEDC0}" name="Output4" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{88F2DAC4-E2C3-4C34-B709-2523E8BE5B1F}" name="Relation_In1_In2" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{3C190E97-FD9A-4F36-8EBF-717B1ECA00B1}" name="Relation_In1_In3" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{043147D8-AE82-457E-8F19-EB4AE9D43B9E}" name="Relation_In1_In4" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{A190E492-7FDF-403D-B8AF-17448A48E47F}" name="Relation_In1_Out1" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{26E8D274-C985-4E20-8920-2BAC0A372552}" name="Relation_Out1_Out2" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{4E0BCAE8-11F8-4D98-AECC-86C8A3C2B5C1}" name="Relation_Out1_Out3" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{3C0369D5-4DD0-4B4B-9480-0C4665C0BC59}" name="Relation_Out1_Out4" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1304,7 +1356,7 @@
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -1323,7 +1375,7 @@
     <tableColumn id="21" xr3:uid="{EC2CC790-C17D-4744-A981-3984808E5B33}" name="vom_cost_Input2"/>
     <tableColumn id="24" xr3:uid="{41B338E4-2058-41E9-8000-97D77450FBC3}" name="vom_cost_Output1"/>
     <tableColumn id="25" xr3:uid="{DDAFCF0A-1EF1-4B7B-9742-01F9FA7A22E5}" name="vom_cost_Output2"/>
-    <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime" dataDxfId="1"/>
+    <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime" dataDxfId="2"/>
     <tableColumn id="30" xr3:uid="{09434E4A-7BF5-4547-9708-EA3F0F7ADC8E}" name="initial_connections_invested_available"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1334,7 +1386,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:K5" totalsRowShown="0">
   <autoFilter ref="A1:K5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="1">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{8C29206C-8DC6-44DB-A8D1-3D5625C277AD}" name="Object_type"/>
@@ -1661,30 +1713,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="10.54296875" customWidth="1"/>
-    <col min="12" max="12" width="12.7265625" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="10.54296875" customWidth="1"/>
+    <col min="13" max="13" width="12.7265625" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C1" t="s">
@@ -1737,7 +1788,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="9" t="s">
         <v>66</v>
       </c>
       <c r="B2" t="s">
@@ -1750,7 +1801,7 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="10" t="s">
         <v>93</v>
       </c>
       <c r="B3" t="s">
@@ -1763,7 +1814,7 @@
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B4" t="s">
@@ -1776,7 +1827,7 @@
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B5" t="s">
@@ -1798,7 +1849,7 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="9" t="s">
         <v>101</v>
       </c>
       <c r="B6" t="s">
@@ -1811,7 +1862,7 @@
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="10" t="s">
         <v>104</v>
       </c>
       <c r="B7" t="s">
@@ -1824,7 +1875,7 @@
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="9" t="s">
         <v>99</v>
       </c>
       <c r="B8" t="s">
@@ -1836,21 +1887,31 @@
       <c r="N8">
         <v>1.4865951742627345E-3</v>
       </c>
+      <c r="O8">
+        <v>0.2</v>
+      </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="10"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="9"/>
+    </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="10"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P11:P12 P2:P8" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P8 P11 Q12" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
       <formula1>"h, D, W, M, Q, Y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1866,7 +1927,7 @@
           <x14:formula1>
             <xm:f>Drop_Down!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B11:B1048576 B1:B8</xm:sqref>
+          <xm:sqref>C12:C1048576 A11 B1:B8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1878,14 +1939,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CABA7C5-6230-4207-9D35-0A95D86E66AC}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1"/>
     <col min="7" max="8" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
adding additional parameter values
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/Products/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/Products/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/Products/ammonia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\Products\ammonia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{51A398C2-2803-4388-96E0-F2CB59F35ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1B88561-2ACF-4BED-8233-B3D3F9BA2DD0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EEA250-A432-4F2C-B286-1C9A375E2C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="-20490" windowWidth="25020" windowHeight="19680" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -530,45 +530,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="28">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1276,6 +1244,38 @@
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1289,15 +1289,11 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:R11" totalsRowShown="0">
   <autoFilter ref="A1:R11" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{88DF4E3A-CD2C-432F-B85D-4C82436680EB}" name="Unit" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{88DF4E3A-CD2C-432F-B85D-4C82436680EB}" name="Unit" dataDxfId="27"/>
     <tableColumn id="40" xr3:uid="{C2CFC5A4-5329-4F74-926A-18CEB18C062C}" name="Object_type"/>
     <tableColumn id="19" xr3:uid="{976E2DCC-BEF9-4E7C-96F4-92D75CC694A2}" name="unit_capacity"/>
     <tableColumn id="35" xr3:uid="{C3887B4E-C4A5-42AB-A92F-97AD44212E95}" name="mean_efficiency"/>
@@ -1312,8 +1308,8 @@
     <tableColumn id="12" xr3:uid="{F1A83AF0-CF23-4B00-9076-4E28DF8DAFD3}" name="fom_cost"/>
     <tableColumn id="21" xr3:uid="{400CD12D-8ADA-4557-B7CA-1464809EAFF0}" name="vom_cost"/>
     <tableColumn id="15" xr3:uid="{3F5A9F9C-E4A0-47A3-8DED-03601A5E69E7}" name="minimum_op_point"/>
-    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="27"/>
-    <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="26"/>
+    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="26"/>
+    <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="25"/>
     <tableColumn id="16" xr3:uid="{5F06ED78-6F41-4BEA-9209-36407E8BCFDC}" name="initial_units_on"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1321,26 +1317,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}" name="Table5" displayName="Table5" ref="A1:Q10" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}" name="Table5" displayName="Table5" ref="A1:Q10" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="A1:Q10" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{2BE3E317-773B-4E82-9035-69A43C6CB21B}" name="Unit" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{22613EE0-390D-4B04-9A9B-6D5554D1C8ED}" name="Object_type" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{54CD83B6-B63A-4ABD-99BD-9ED391BFB078}" name="Input1" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{F183F72C-A42E-4046-9CA2-B23C4DD3765C}" name="Input2" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{CA468CF3-FA3A-4DED-8C1A-ED8385FD2167}" name="Input3" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{6C9174ED-453E-45B1-B2C9-DC69B7CB535A}" name="Input4" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{513A63E4-7BE3-4AF5-AC5E-11EB4AF0D7AD}" name="Output1" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{4623E738-60A2-497B-BD61-91A608129A61}" name="Output2" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{5596B30B-5CDD-4E38-8C15-9C5F774E9B1F}" name="Output3" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{CD6FCAF1-2543-4CF8-99F5-E24DBA2DEDC0}" name="Output4" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{88F2DAC4-E2C3-4C34-B709-2523E8BE5B1F}" name="Relation_In1_In2" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{3C190E97-FD9A-4F36-8EBF-717B1ECA00B1}" name="Relation_In1_In3" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{043147D8-AE82-457E-8F19-EB4AE9D43B9E}" name="Relation_In1_In4" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{A190E492-7FDF-403D-B8AF-17448A48E47F}" name="Relation_In1_Out1" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{26E8D274-C985-4E20-8920-2BAC0A372552}" name="Relation_Out1_Out2" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{4E0BCAE8-11F8-4D98-AECC-86C8A3C2B5C1}" name="Relation_Out1_Out3" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{3C0369D5-4DD0-4B4B-9480-0C4665C0BC59}" name="Relation_Out1_Out4" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{2BE3E317-773B-4E82-9035-69A43C6CB21B}" name="Unit" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{22613EE0-390D-4B04-9A9B-6D5554D1C8ED}" name="Object_type" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{54CD83B6-B63A-4ABD-99BD-9ED391BFB078}" name="Input1" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{F183F72C-A42E-4046-9CA2-B23C4DD3765C}" name="Input2" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{CA468CF3-FA3A-4DED-8C1A-ED8385FD2167}" name="Input3" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{6C9174ED-453E-45B1-B2C9-DC69B7CB535A}" name="Input4" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{513A63E4-7BE3-4AF5-AC5E-11EB4AF0D7AD}" name="Output1" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{4623E738-60A2-497B-BD61-91A608129A61}" name="Output2" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{5596B30B-5CDD-4E38-8C15-9C5F774E9B1F}" name="Output3" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{CD6FCAF1-2543-4CF8-99F5-E24DBA2DEDC0}" name="Output4" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{88F2DAC4-E2C3-4C34-B709-2523E8BE5B1F}" name="Relation_In1_In2" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{3C190E97-FD9A-4F36-8EBF-717B1ECA00B1}" name="Relation_In1_In3" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{043147D8-AE82-457E-8F19-EB4AE9D43B9E}" name="Relation_In1_In4" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{A190E492-7FDF-403D-B8AF-17448A48E47F}" name="Relation_In1_Out1" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{26E8D274-C985-4E20-8920-2BAC0A372552}" name="Relation_Out1_Out2" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{4E0BCAE8-11F8-4D98-AECC-86C8A3C2B5C1}" name="Relation_Out1_Out3" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{3C0369D5-4DD0-4B4B-9480-0C4665C0BC59}" name="Relation_Out1_Out4" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1356,7 +1352,7 @@
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -1375,7 +1371,7 @@
     <tableColumn id="21" xr3:uid="{EC2CC790-C17D-4744-A981-3984808E5B33}" name="vom_cost_Input2"/>
     <tableColumn id="24" xr3:uid="{41B338E4-2058-41E9-8000-97D77450FBC3}" name="vom_cost_Output1"/>
     <tableColumn id="25" xr3:uid="{DDAFCF0A-1EF1-4B7B-9742-01F9FA7A22E5}" name="vom_cost_Output2"/>
-    <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime" dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime" dataDxfId="1"/>
     <tableColumn id="30" xr3:uid="{09434E4A-7BF5-4547-9708-EA3F0F7ADC8E}" name="initial_connections_invested_available"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1386,7 +1382,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:K5" totalsRowShown="0">
   <autoFilter ref="A1:K5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{8C29206C-8DC6-44DB-A8D1-3D5625C277AD}" name="Object_type"/>
@@ -1713,7 +1709,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1871,6 +1869,9 @@
       <c r="C7" t="s">
         <v>106</v>
       </c>
+      <c r="O7">
+        <v>0.2</v>
+      </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="2"/>
     </row>
@@ -1886,9 +1887,6 @@
       </c>
       <c r="N8">
         <v>1.4865951742627345E-3</v>
-      </c>
-      <c r="O8">
-        <v>0.2</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>

</xml_diff>

<commit_message>
updating values for ammonia
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/Products/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/Products/ammonia/Model_Data_Base_ammonia_4_InOutputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\Products\ammonia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EEA250-A432-4F2C-B286-1C9A375E2C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE50409-AE50-494F-8D03-B44D3C245BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -1709,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1856,6 +1856,9 @@
       <c r="C6" t="s">
         <v>105</v>
       </c>
+      <c r="O6">
+        <v>0.4</v>
+      </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
@@ -1868,6 +1871,15 @@
       </c>
       <c r="C7" t="s">
         <v>106</v>
+      </c>
+      <c r="E7">
+        <v>24</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
       </c>
       <c r="O7">
         <v>0.2</v>
@@ -2262,8 +2274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E25:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>